<commit_message>
added content to the README.md file
</commit_message>
<xml_diff>
--- a/Channel_crosstalk.xlsx
+++ b/Channel_crosstalk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pwilmart/Box Sync/Github_misc/meetings_presentations/TMT_channel_cross_talk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AA23C6-2EF4-2648-9A98-E5EEC94E9819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B0B137-6237-FB41-9E00-F118F183F345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="31860" windowHeight="28300" activeTab="2" xr2:uid="{A9539795-6B07-D548-A2ED-7E776BC4A3B1}"/>
   </bookViews>
@@ -1517,7 +1517,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2000" b="1"/>
-              <a:t>Reporter Ion Releative Intensities with Cross Talk</a:t>
+              <a:t>Reporter Ion Relative Intensities with Cross Talk</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -10025,7 +10025,7 @@
   <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T51" sqref="T51"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>